<commit_message>
MOSIP-32620 Added spa language in language and template file format table
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/language.xlsx
+++ b/mosip_master/xlsx/language.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674CF7A0-5227-46BB-BCF6-C6388E1DC0B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649DD1E9-029F-407A-B6DC-F61FA172D96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>code</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Tamil</t>
+  </si>
+  <si>
+    <t>spa</t>
+  </si>
+  <si>
+    <t>Spanish</t>
   </si>
 </sst>
 </file>
@@ -165,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -174,7 +180,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,16 +494,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="8.44140625" style="1"/>
+    <col min="5" max="5" width="8.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -515,41 +522,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -566,7 +573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -583,7 +590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -600,7 +607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -614,6 +621,23 @@
         <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>